<commit_message>
Modificación Tabla de Casos de Prueba Excel. Carmelo
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juane\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Escritorio\GIT\Semillero2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8870A9-1F90-4E55-B616-3B15D4A8C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2AF6EA-F849-4E05-9B24-9C9B36E49916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{6675418A-09A9-40FA-8F0D-C76F72AF9085}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6675418A-09A9-40FA-8F0D-C76F72AF9085}"/>
   </bookViews>
   <sheets>
     <sheet name="CASOS DE PRUEBAS " sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="134">
   <si>
     <t>TIPO DE ESCENARIO</t>
   </si>
@@ -195,12 +195,6 @@
   </si>
   <si>
     <t>CASOS DE PRUEBA</t>
-  </si>
-  <si>
-    <t>1. Seleccionar "Cargar videos".
-2. Seleccionar 2 videos en formato mp4 con tamaño mayor a 100Mb en algun video.
-3. Seleccionar 2 videos en un formato diferente a mp4 en al menos un video.
-4. Seleccionar 3 o más videos en cualquier formato.</t>
   </si>
   <si>
     <t xml:space="preserve">- Caracteres de texto del teclado.
@@ -260,6 +254,268 @@
 4. Ingresar numeros.
 5. Ingresar caracteres especiales.
 </t>
+  </si>
+  <si>
+    <t>EQUIPO 2</t>
+  </si>
+  <si>
+    <t>CP010</t>
+  </si>
+  <si>
+    <t>Validar rechazo campo para publicar en el blog.</t>
+  </si>
+  <si>
+    <t>Comprobar que el usuario no pueda publicar contenido con emojis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar al blog.
+2. Click en el espacio para publicar contenido.
+3. Ingresar emojis.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Emojis ingresados.
+</t>
+  </si>
+  <si>
+    <t>- Mensaje de impedimento por ingreso datos no permitido</t>
+  </si>
+  <si>
+    <t>Exitoso, el sistema no permite ingresar datos no validos</t>
+  </si>
+  <si>
+    <t>CP011</t>
+  </si>
+  <si>
+    <t>Validar publicación de enlaces web.</t>
+  </si>
+  <si>
+    <t>Comprobar la publicación de enlaces web en el blog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Escribir una dirección web de dominio ".com", ".net"  que se desea publicar.
+2. Copiar y pegar la dirección web de dominio ".com", ".net"  que se desea publicar.
+</t>
+  </si>
+  <si>
+    <t>- Dirección web de dominio ".com",  y ".net".</t>
+  </si>
+  <si>
+    <t>- Dirección web ingresada</t>
+  </si>
+  <si>
+    <t>CP012</t>
+  </si>
+  <si>
+    <t>Validar rechazo de publicación de enlaces web</t>
+  </si>
+  <si>
+    <t>Comprobar que no se realice la publicación de enlaces no permitidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Escribir una dirección web de dominio ".gov" u otro dominio diferente a ".com" o ".net" que se desea publicar.
+2. Copiar y pegar la dirección web  de otro dominio diferente a ".com" o ".net" que se desea publicar.
+</t>
+  </si>
+  <si>
+    <t>- Dirección web de dominio ".gov" u otro dominio diferente a ".com" o ".net".</t>
+  </si>
+  <si>
+    <t>- Mensaje de impedimento de publicación por dominio o contenido no admitido.</t>
+  </si>
+  <si>
+    <t>CP013</t>
+  </si>
+  <si>
+    <t>Validar edición de estilo y estrutura de texto en la entrada del blog.</t>
+  </si>
+  <si>
+    <t>Comprobar que el usuario pueda darle formato al texto que desea publicar</t>
+  </si>
+  <si>
+    <t>1. Ingresar un texto.
+2. Aplicar negrita al texto.
+3. Aplicar cursiva al texto.
+4. Aplicar subrayado al texto.
+5. Cambiar color al texto.
+6. Aumentar y disminuir tamaño al texto. 
+7. Alinear texto (centro, derecha, izquierda)</t>
+  </si>
+  <si>
+    <t>- Texto ingresado.</t>
+  </si>
+  <si>
+    <t>- Texto en negrita.
+- Texto en cursiva.
+- Texto subrayado.
+- Texto a color.
+- Texto con más o menos tamaño.
+- Texto alineado.</t>
+  </si>
+  <si>
+    <t>Exitoso, el sistema permite publicar texto.</t>
+  </si>
+  <si>
+    <t>CP014</t>
+  </si>
+  <si>
+    <t>Validar publicación del contenido de la entrada del Blog en redes sociales</t>
+  </si>
+  <si>
+    <t>Comprobar que el sistema permita compartir una publicación en redes sociales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Elegir la publicación a compartir.
+2. Click en compartir a redes sociales.
+3. Click en compartir a través de Facebook.
+4. Ingresar los datos del usuario (Usuario y contraseña) y click en compartir.
+5. Click en compartir a través de Instagram.
+6. Ingresar los datos del usuario (Usuario y contraseña) y click en compartir.
+7. Click en compartir a través de Twitter.
+8. Ingresar los datos del usuario (Usuario y contraseña) y click en compartir. 
+9.  Click en compartir a través de LinkedIn.
+10. Ingresar los datos del usuario (Usuario y contraseña) y click en compartir. </t>
+  </si>
+  <si>
+    <t>- Publicación que se desea compartir.</t>
+  </si>
+  <si>
+    <t>- Publicación a compartir.</t>
+  </si>
+  <si>
+    <t>Exitoso, el sistema permite compartir la publicación a redes sociales</t>
+  </si>
+  <si>
+    <t>CP015</t>
+  </si>
+  <si>
+    <t>Validar rechazo en publicación del contenido de la entrada del Blog en redes sociales</t>
+  </si>
+  <si>
+    <t>Comprobar que el sistema permita no permita compartir una publicación en redes sociales sin el procedimiento correcto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Elegir la publicación a compartir.
+2. Click en compartir a redes sociales.
+3. Click en compartir a través de Facebook.
+4. No ingresar los datos del usuario (Usuario y contraseña) y click en compartir.
+5. Click en compartir a través de Instagram.
+6. No ingresar los datos del usuario (Usuario y contraseña) y click en compartir.
+7. Click en compartir a través de Twitter.
+8. No ingresar los datos del usuario (Usuario y contraseña) y click en compartir. 
+9.  Click en compartir a través de LinkedIn.
+10. No ingresar los datos del usuario (Usuario y contraseña) y click en compartir. </t>
+  </si>
+  <si>
+    <t>- Mensaje de impedimento a compartir por no ingresar datos del usuario.</t>
+  </si>
+  <si>
+    <t>Exitoso, el sistema no permite compartir la publicación a redes sociales</t>
+  </si>
+  <si>
+    <t>CP016</t>
+  </si>
+  <si>
+    <t>Validar la impresión del contenido de la Entrada publicación del blog</t>
+  </si>
+  <si>
+    <t>Comprobar que el sistema permita imprimir una publicación.</t>
+  </si>
+  <si>
+    <t>1. Elegir una publicación con texto (incluídas direcciones web) o texto + imágenes para imprimir.
+2. Conectar la impresora con el ordenador.
+3. Click en imprimir.
+4. Seleccionar impresora.
+5. Aplicar formato deseado.
+6. Click en aceptar.</t>
+  </si>
+  <si>
+    <t>- Publicación que se desea imprimir.</t>
+  </si>
+  <si>
+    <t>- Interfaz de impresión.
+- Vista previa de la impresión.</t>
+  </si>
+  <si>
+    <t>Exitoso, el sistema permite imprimir el contenido de una publicación.</t>
+  </si>
+  <si>
+    <t>CP017</t>
+  </si>
+  <si>
+    <t>Validar rechazo de la impresión del contenido de la Entrada publicación del blog.</t>
+  </si>
+  <si>
+    <t>Comprobar que el sistema no permita imprimir publicaciones con videos.</t>
+  </si>
+  <si>
+    <t>1. Elegir una publicación con uno o dos videos para imprimir.
+2. Conectar la impresora con el ordenador.
+3. Click en imprimir.
+4. Seleccionar impresora.
+5. Aplicar formato deseado.
+6. Click en aceptar.</t>
+  </si>
+  <si>
+    <t>- Mensaje de impedimento indicando que el contenido no se puede imprimir.</t>
+  </si>
+  <si>
+    <t>Exitoso, el sistema no permite imprimir un video.</t>
+  </si>
+  <si>
+    <t>CP018</t>
+  </si>
+  <si>
+    <t>Validar el envio de una publicación por correo eletrónico.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprobar que el sistema permita enviar una publicación por correo electrónico </t>
+  </si>
+  <si>
+    <t>1. Elegir la publicación a enviar por correo.
+2. Click en "Enviar vía correo electrónico".
+3. Ingresar correo electrónico del Remitente.
+4. Ingresar correo electrónico del Destinatario.
+5. Ingresar Asunto (este campo es opcional)
+6. Click en enviar.</t>
+  </si>
+  <si>
+    <t>- Publicación a enviar por correo electrónico.</t>
+  </si>
+  <si>
+    <t>- Vista previa del contenido de la publicación a enviar.</t>
+  </si>
+  <si>
+    <t>Exitoso, el sistema permite el envio de una publicación vía correo electrónico.</t>
+  </si>
+  <si>
+    <t>CP019</t>
+  </si>
+  <si>
+    <t>Validar el rechazo de  enviar una publicación por correo eletrónico.</t>
+  </si>
+  <si>
+    <t>Comprobar que el sistema No permita enviar una publicación por correo electrónico sin el procedimiento correcto.</t>
+  </si>
+  <si>
+    <t>1. Elegir la publicación a enviar por correo.
+2. Click en "Enviar vía correo electrónico".
+3. No ingresar correo electrónico del Remitente.
+4. No Ingresar correo electrónico del Destinatario.
+5. Ingresar Asunto (este campo es opcional)
+6. Click en enviar.</t>
+  </si>
+  <si>
+    <t>- Mensaje de impedimento por falta de requerimientos obligatorios.</t>
+  </si>
+  <si>
+    <t>Exitoso, el sistema no permite el envio de la publicación vía correo electrónico..</t>
+  </si>
+  <si>
+    <t>1. Seleccionar "Insertar videos".
+2. Seleccionar 2 videos en formato mp4 con tamaño mayor a 100Mb en algun video.
+3. Seleccionar 2 videos en un formato diferente a mp4 en al menos un video.
+4. Seleccionar 3 o más videos en cualquier formato.</t>
   </si>
 </sst>
 </file>
@@ -631,15 +887,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -655,6 +902,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1026,30 +1282,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C99C55-88B4-477C-A0D3-7EA5549F9807}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.81640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="31.26953125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.26953125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="11.453125" style="3"/>
+    <col min="1" max="1" width="1.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>53</v>
       </c>
       <c r="E1" s="12"/>
@@ -1059,11 +1315,13 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="24"/>
+      <c r="D2" s="24" t="s">
+        <v>67</v>
+      </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -1071,7 +1329,7 @@
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1084,21 +1342,21 @@
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27"/>
-    </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="33"/>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="22" t="s">
         <v>1</v>
@@ -1128,7 +1386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="66.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="66.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="6" t="s">
         <v>8</v>
@@ -1143,7 +1401,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>20</v>
@@ -1158,7 +1416,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="6" t="s">
         <v>10</v>
@@ -1173,7 +1431,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>20</v>
@@ -1188,7 +1446,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="6" t="s">
         <v>11</v>
@@ -1203,7 +1461,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>51</v>
@@ -1212,13 +1470,13 @@
         <v>9</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" ht="117" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
         <v>12</v>
@@ -1233,7 +1491,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>52</v>
@@ -1248,7 +1506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
         <v>13</v>
@@ -1263,7 +1521,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>35</v>
@@ -1278,7 +1536,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="6" t="s">
         <v>14</v>
@@ -1293,7 +1551,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>35</v>
@@ -1308,7 +1566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" ht="52" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="6" t="s">
         <v>15</v>
@@ -1323,7 +1581,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>47</v>
@@ -1338,13 +1596,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="2" customFormat="1" ht="91" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>30</v>
@@ -1353,7 +1611,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>46</v>
@@ -1368,25 +1626,25 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="2" customFormat="1" ht="91" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="E14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>67</v>
-      </c>
       <c r="G14" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>9</v>
@@ -1398,123 +1656,303 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" s="2" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="2" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" s="14" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="1:10" s="29" customFormat="1" ht="181" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="6"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" s="2" customFormat="1" ht="182.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="14" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="26" customFormat="1" ht="180.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="2" customFormat="1" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10" s="2" customFormat="1" ht="119" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="2" customFormat="1" ht="119.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" s="2" customFormat="1" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="2" customFormat="1" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="2" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="7"/>
-    </row>
-    <row r="24" spans="1:10" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="2" customFormat="1" ht="128.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="11"/>
+      <c r="B24" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>